<commit_message>
changed analysis R script so that files don't need to be moved around
</commit_message>
<xml_diff>
--- a/data/01 application country names per year.xlsx
+++ b/data/01 application country names per year.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t>project_year</t>
   </si>
@@ -68,132 +68,132 @@
     <t>Cameroon</t>
   </si>
   <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Palestine, State of</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Korea, Republic of</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>Timor-Leste</t>
+  </si>
+  <si>
+    <t>Lao People's Democratic Republic</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
     <t>Papua New Guinea</t>
   </si>
   <si>
-    <t>Lesotho</t>
-  </si>
-  <si>
-    <t>Israel</t>
-  </si>
-  <si>
-    <t>Uganda</t>
-  </si>
-  <si>
-    <t>Egypt</t>
-  </si>
-  <si>
-    <t>Ethiopia</t>
-  </si>
-  <si>
-    <t>Cambodia</t>
-  </si>
-  <si>
-    <t>Philippines</t>
-  </si>
-  <si>
-    <t>Pakistan</t>
-  </si>
-  <si>
-    <t>Singapore</t>
-  </si>
-  <si>
-    <t>Palestine, State of</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Malawi</t>
-  </si>
-  <si>
-    <t>Iraq</t>
-  </si>
-  <si>
-    <t>Afghanistan</t>
-  </si>
-  <si>
-    <t>Zimbabwe</t>
-  </si>
-  <si>
-    <t>Korea, Republic of</t>
-  </si>
-  <si>
-    <t>Mali</t>
-  </si>
-  <si>
-    <t>Bangladesh</t>
-  </si>
-  <si>
-    <t>Bhutan</t>
-  </si>
-  <si>
-    <t>Timor-Leste</t>
-  </si>
-  <si>
-    <t>Lao People's Democratic Republic</t>
-  </si>
-  <si>
-    <t>Thailand</t>
-  </si>
-  <si>
-    <t>Morocco</t>
-  </si>
-  <si>
-    <t>Malaysia</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>Sri Lanka</t>
-  </si>
-  <si>
-    <t>Liberia</t>
-  </si>
-  <si>
-    <t>Central African Republic</t>
-  </si>
-  <si>
-    <t>Mauritania</t>
-  </si>
-  <si>
-    <t>Burundi</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>Kyrgyzstan</t>
-  </si>
-  <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>Lebanon</t>
-  </si>
-  <si>
-    <t>Sierra Leone</t>
-  </si>
-  <si>
-    <t>Somalia</t>
-  </si>
-  <si>
-    <t>2012</t>
-  </si>
-  <si>
-    <t>Tunisia</t>
-  </si>
-  <si>
     <t>Sudan</t>
   </si>
   <si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>Maldives</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>New Zealand</t>
@@ -1121,458 +1124,458 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" t="s">
         <v>58</v>
-      </c>
-      <c r="B60" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>59</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B63" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B64" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B65" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B66" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B69" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B70" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B71" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B72" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B73" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B74" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B75" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B76" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B77" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B78" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B79" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B80" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B81" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B82" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B83" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B84" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B85" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B86" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B87" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B89" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B90" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B91" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B92" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B93" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B94" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B95" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B96" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B97" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B98" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B99" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B100" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B101" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B102" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B103" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B104" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B105" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B106" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B107" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B108" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B109" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B110" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B111" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B112" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113">
@@ -1580,7 +1583,7 @@
         <v>72</v>
       </c>
       <c r="B113" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
     </row>
     <row r="114">
@@ -1588,7 +1591,7 @@
         <v>72</v>
       </c>
       <c r="B114" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
     </row>
     <row r="115">
@@ -1596,7 +1599,7 @@
         <v>72</v>
       </c>
       <c r="B115" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116">
@@ -1604,7 +1607,7 @@
         <v>72</v>
       </c>
       <c r="B116" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
     <row r="117">
@@ -1612,7 +1615,7 @@
         <v>72</v>
       </c>
       <c r="B117" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118">
@@ -1620,7 +1623,7 @@
         <v>72</v>
       </c>
       <c r="B118" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
     </row>
     <row r="119">
@@ -1628,7 +1631,7 @@
         <v>72</v>
       </c>
       <c r="B119" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
     <row r="120">
@@ -1636,7 +1639,7 @@
         <v>72</v>
       </c>
       <c r="B120" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
     </row>
     <row r="121">
@@ -1644,7 +1647,7 @@
         <v>72</v>
       </c>
       <c r="B121" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
     </row>
     <row r="122">
@@ -1652,7 +1655,7 @@
         <v>72</v>
       </c>
       <c r="B122" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123">
@@ -1660,7 +1663,7 @@
         <v>72</v>
       </c>
       <c r="B123" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="124">
@@ -1668,7 +1671,7 @@
         <v>72</v>
       </c>
       <c r="B124" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="125">
@@ -1684,7 +1687,7 @@
         <v>72</v>
       </c>
       <c r="B126" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
     </row>
     <row r="127">
@@ -1692,7 +1695,7 @@
         <v>72</v>
       </c>
       <c r="B127" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128">
@@ -1700,7 +1703,7 @@
         <v>72</v>
       </c>
       <c r="B128" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
     </row>
     <row r="129">
@@ -1708,7 +1711,7 @@
         <v>72</v>
       </c>
       <c r="B129" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="130">
@@ -1716,7 +1719,7 @@
         <v>72</v>
       </c>
       <c r="B130" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="131">
@@ -1724,7 +1727,7 @@
         <v>72</v>
       </c>
       <c r="B131" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
     </row>
     <row r="132">
@@ -1732,7 +1735,7 @@
         <v>72</v>
       </c>
       <c r="B132" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
     </row>
     <row r="133">
@@ -1740,7 +1743,7 @@
         <v>72</v>
       </c>
       <c r="B133" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
     </row>
     <row r="134">
@@ -1748,7 +1751,7 @@
         <v>72</v>
       </c>
       <c r="B134" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="135">
@@ -1756,7 +1759,7 @@
         <v>72</v>
       </c>
       <c r="B135" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="136">
@@ -1772,7 +1775,7 @@
         <v>72</v>
       </c>
       <c r="B137" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="138">
@@ -1780,7 +1783,7 @@
         <v>72</v>
       </c>
       <c r="B138" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139">
@@ -1788,7 +1791,7 @@
         <v>72</v>
       </c>
       <c r="B139" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
     </row>
     <row r="140">
@@ -1796,7 +1799,7 @@
         <v>72</v>
       </c>
       <c r="B140" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
     </row>
     <row r="141">
@@ -1804,7 +1807,7 @@
         <v>72</v>
       </c>
       <c r="B141" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="142">
@@ -1812,7 +1815,7 @@
         <v>72</v>
       </c>
       <c r="B142" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="143">
@@ -1820,7 +1823,7 @@
         <v>72</v>
       </c>
       <c r="B143" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
     </row>
     <row r="144">
@@ -1828,7 +1831,7 @@
         <v>72</v>
       </c>
       <c r="B144" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
     <row r="145">
@@ -1836,7 +1839,7 @@
         <v>72</v>
       </c>
       <c r="B145" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
     </row>
     <row r="146">
@@ -1844,7 +1847,7 @@
         <v>72</v>
       </c>
       <c r="B146" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
     </row>
     <row r="147">
@@ -1852,7 +1855,7 @@
         <v>72</v>
       </c>
       <c r="B147" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
     </row>
     <row r="148">
@@ -1860,7 +1863,7 @@
         <v>72</v>
       </c>
       <c r="B148" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="149">
@@ -1868,7 +1871,7 @@
         <v>72</v>
       </c>
       <c r="B149" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
     </row>
     <row r="150">
@@ -1876,7 +1879,7 @@
         <v>72</v>
       </c>
       <c r="B150" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
     </row>
     <row r="151">
@@ -1884,7 +1887,7 @@
         <v>72</v>
       </c>
       <c r="B151" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
     </row>
     <row r="152">
@@ -1892,7 +1895,7 @@
         <v>72</v>
       </c>
       <c r="B152" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="153">
@@ -1900,7 +1903,7 @@
         <v>72</v>
       </c>
       <c r="B153" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
     </row>
     <row r="154">
@@ -1908,7 +1911,7 @@
         <v>72</v>
       </c>
       <c r="B154" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="155">
@@ -1916,7 +1919,7 @@
         <v>72</v>
       </c>
       <c r="B155" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="156">
@@ -1924,7 +1927,7 @@
         <v>72</v>
       </c>
       <c r="B156" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="157">
@@ -1932,7 +1935,7 @@
         <v>72</v>
       </c>
       <c r="B157" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="158">
@@ -1940,7 +1943,7 @@
         <v>72</v>
       </c>
       <c r="B158" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="159">
@@ -1948,7 +1951,7 @@
         <v>72</v>
       </c>
       <c r="B159" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="160">
@@ -1972,7 +1975,7 @@
         <v>72</v>
       </c>
       <c r="B162" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="163">
@@ -1980,7 +1983,7 @@
         <v>72</v>
       </c>
       <c r="B163" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="164">
@@ -1988,7 +1991,7 @@
         <v>72</v>
       </c>
       <c r="B164" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="165">
@@ -2004,7 +2007,7 @@
         <v>72</v>
       </c>
       <c r="B166" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="167">
@@ -2012,7 +2015,7 @@
         <v>72</v>
       </c>
       <c r="B167" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="168">
@@ -2020,7 +2023,7 @@
         <v>72</v>
       </c>
       <c r="B168" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="169">
@@ -2028,7 +2031,7 @@
         <v>72</v>
       </c>
       <c r="B169" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="170">
@@ -2036,7 +2039,7 @@
         <v>72</v>
       </c>
       <c r="B170" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="171">
@@ -2044,7 +2047,7 @@
         <v>72</v>
       </c>
       <c r="B171" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="172">
@@ -2052,7 +2055,7 @@
         <v>72</v>
       </c>
       <c r="B172" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="173">
@@ -2060,7 +2063,7 @@
         <v>72</v>
       </c>
       <c r="B173" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="174">
@@ -2068,7 +2071,7 @@
         <v>72</v>
       </c>
       <c r="B174" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="175">
@@ -2076,7 +2079,7 @@
         <v>72</v>
       </c>
       <c r="B175" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="176">
@@ -2084,7 +2087,7 @@
         <v>72</v>
       </c>
       <c r="B176" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="177">
@@ -2092,7 +2095,7 @@
         <v>72</v>
       </c>
       <c r="B177" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="178">
@@ -2116,7 +2119,7 @@
         <v>72</v>
       </c>
       <c r="B180" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="181">
@@ -2124,7 +2127,7 @@
         <v>72</v>
       </c>
       <c r="B181" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="182">
@@ -2132,7 +2135,7 @@
         <v>72</v>
       </c>
       <c r="B182" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="183">
@@ -2140,7 +2143,7 @@
         <v>72</v>
       </c>
       <c r="B183" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="184">
@@ -2148,7 +2151,7 @@
         <v>72</v>
       </c>
       <c r="B184" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="185">
@@ -2156,12 +2159,12 @@
         <v>72</v>
       </c>
       <c r="B185" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B186" t="s">
         <v>4</v>
@@ -2169,47 +2172,47 @@
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B187" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B188" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B189" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B190" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B191" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B192" t="s">
         <v>3</v>
@@ -2217,15 +2220,15 @@
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B193" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B194" t="s">
         <v>7</v>
@@ -2233,15 +2236,15 @@
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B195" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B196" t="s">
         <v>12</v>
@@ -2249,7 +2252,7 @@
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B197" t="s">
         <v>10</v>
@@ -2257,7 +2260,7 @@
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B198" t="s">
         <v>17</v>
@@ -2265,15 +2268,15 @@
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B199" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B200" t="s">
         <v>15</v>
@@ -2281,15 +2284,15 @@
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B201" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B202" t="s">
         <v>13</v>
@@ -2297,7 +2300,7 @@
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B203" t="s">
         <v>6</v>
@@ -2305,15 +2308,15 @@
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B204" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B205" t="s">
         <v>69</v>
@@ -2321,47 +2324,47 @@
     </row>
     <row r="206">
       <c r="A206" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B206" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B207" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B208" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B209" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B210" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B211" t="s">
         <v>11</v>
@@ -2369,15 +2372,15 @@
     </row>
     <row r="212">
       <c r="A212" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B212" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B213" t="s">
         <v>61</v>
@@ -2385,31 +2388,31 @@
     </row>
     <row r="214">
       <c r="A214" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B214" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B215" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B216" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B217" t="s">
         <v>71</v>
@@ -2417,23 +2420,23 @@
     </row>
     <row r="218">
       <c r="A218" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B218" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B219" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B220" t="s">
         <v>16</v>
@@ -2441,31 +2444,31 @@
     </row>
     <row r="221">
       <c r="A221" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B221" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B222" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B223" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B224" t="s">
         <v>78</v>
@@ -2473,7 +2476,7 @@
     </row>
     <row r="225">
       <c r="A225" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B225" t="s">
         <v>67</v>
@@ -2481,15 +2484,15 @@
     </row>
     <row r="226">
       <c r="A226" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B226" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B227" t="s">
         <v>5</v>
@@ -2497,39 +2500,39 @@
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B228" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B229" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B230" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B231" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B232" t="s">
         <v>79</v>
@@ -2537,15 +2540,15 @@
     </row>
     <row r="233">
       <c r="A233" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B233" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B234" t="s">
         <v>14</v>
@@ -2553,63 +2556,63 @@
     </row>
     <row r="235">
       <c r="A235" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B235" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B236" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B237" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B238" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B239" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B240" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B241" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B242" t="s">
         <v>60</v>
@@ -2617,15 +2620,15 @@
     </row>
     <row r="243">
       <c r="A243" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B243" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B244" t="s">
         <v>8</v>
@@ -2633,63 +2636,63 @@
     </row>
     <row r="245">
       <c r="A245" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B245" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B246" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B247" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B248" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B249" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B250" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B251" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B252" t="s">
         <v>63</v>
@@ -2697,15 +2700,15 @@
     </row>
     <row r="253">
       <c r="A253" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B253" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B254" t="s">
         <v>12</v>
@@ -2713,39 +2716,39 @@
     </row>
     <row r="255">
       <c r="A255" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B255" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B256" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B257" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B258" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B259" t="s">
         <v>11</v>
@@ -2753,15 +2756,15 @@
     </row>
     <row r="260">
       <c r="A260" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B260" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B261" t="s">
         <v>17</v>
@@ -2769,15 +2772,15 @@
     </row>
     <row r="262">
       <c r="A262" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B262" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B263" t="s">
         <v>79</v>
@@ -2785,7 +2788,7 @@
     </row>
     <row r="264">
       <c r="A264" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B264" t="s">
         <v>67</v>
@@ -2793,7 +2796,7 @@
     </row>
     <row r="265">
       <c r="A265" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B265" t="s">
         <v>8</v>
@@ -2801,15 +2804,15 @@
     </row>
     <row r="266">
       <c r="A266" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B266" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B267" t="s">
         <v>3</v>
@@ -2817,199 +2820,199 @@
     </row>
     <row r="268">
       <c r="A268" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B268" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B269" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B270" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B271" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B272" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B273" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B274" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B275" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B276" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B277" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B278" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B279" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B280" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B281" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B282" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B283" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B284" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B285" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B286" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B287" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B288" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B289" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B290" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B291" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B292" t="s">
         <v>16</v>
@@ -3017,7 +3020,7 @@
     </row>
     <row r="293">
       <c r="A293" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B293" t="s">
         <v>14</v>
@@ -3025,15 +3028,15 @@
     </row>
     <row r="294">
       <c r="A294" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B294" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B295" t="s">
         <v>65</v>
@@ -3041,23 +3044,23 @@
     </row>
     <row r="296">
       <c r="A296" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B296" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B297" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B298" t="s">
         <v>78</v>
@@ -3065,74 +3068,74 @@
     </row>
     <row r="299">
       <c r="A299" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B299" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B300" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B301" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B302" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B303" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B304" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="s">
+        <v>106</v>
+      </c>
+      <c r="B305" t="s">
         <v>105</v>
-      </c>
-      <c r="B305" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B306" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B307" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran analysis R code
</commit_message>
<xml_diff>
--- a/data/01 application country names per year.xlsx
+++ b/data/01 application country names per year.xlsx
@@ -200,28 +200,28 @@
     <t>Senegal</t>
   </si>
   <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Solomon Islands</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
     <t>Norway</t>
   </si>
   <si>
-    <t>Yemen</t>
-  </si>
-  <si>
-    <t>Namibia</t>
-  </si>
-  <si>
-    <t>Mozambique</t>
-  </si>
-  <si>
-    <t>Solomon Islands</t>
+    <t>Iran, Islamic Republic of</t>
   </si>
   <si>
     <t>Madagascar</t>
-  </si>
-  <si>
-    <t>Botswana</t>
-  </si>
-  <si>
-    <t>Iran, Islamic Republic of</t>
   </si>
   <si>
     <t>Korea, Democratic People's Republic of</t>
@@ -1391,7 +1391,7 @@
         <v>57</v>
       </c>
       <c r="B89" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90">
@@ -1399,7 +1399,7 @@
         <v>57</v>
       </c>
       <c r="B90" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
     </row>
     <row r="91">
@@ -1407,7 +1407,7 @@
         <v>57</v>
       </c>
       <c r="B91" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92">
@@ -1415,7 +1415,7 @@
         <v>57</v>
       </c>
       <c r="B92" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="93">
@@ -1423,7 +1423,7 @@
         <v>57</v>
       </c>
       <c r="B93" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="94">
@@ -1431,7 +1431,7 @@
         <v>57</v>
       </c>
       <c r="B94" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="95">
@@ -1439,7 +1439,7 @@
         <v>57</v>
       </c>
       <c r="B95" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
     </row>
     <row r="96">
@@ -1455,7 +1455,7 @@
         <v>57</v>
       </c>
       <c r="B97" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
     </row>
     <row r="98">
@@ -1463,7 +1463,7 @@
         <v>57</v>
       </c>
       <c r="B98" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row r="99">
@@ -1471,7 +1471,7 @@
         <v>57</v>
       </c>
       <c r="B99" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100">
@@ -1479,7 +1479,7 @@
         <v>57</v>
       </c>
       <c r="B100" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="101">
@@ -1487,7 +1487,7 @@
         <v>57</v>
       </c>
       <c r="B101" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102">
@@ -1495,7 +1495,7 @@
         <v>57</v>
       </c>
       <c r="B102" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
     </row>
     <row r="103">
@@ -1503,7 +1503,7 @@
         <v>57</v>
       </c>
       <c r="B103" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="104">
@@ -1511,7 +1511,7 @@
         <v>57</v>
       </c>
       <c r="B104" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
     <row r="105">
@@ -1519,7 +1519,7 @@
         <v>57</v>
       </c>
       <c r="B105" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="106">
@@ -1527,7 +1527,7 @@
         <v>57</v>
       </c>
       <c r="B106" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="107">
@@ -1535,7 +1535,7 @@
         <v>57</v>
       </c>
       <c r="B107" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
     </row>
     <row r="108">
@@ -1543,7 +1543,7 @@
         <v>57</v>
       </c>
       <c r="B108" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="109">
@@ -1687,7 +1687,7 @@
         <v>72</v>
       </c>
       <c r="B126" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="127">
@@ -1767,7 +1767,7 @@
         <v>72</v>
       </c>
       <c r="B136" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="137">
@@ -1791,7 +1791,7 @@
         <v>72</v>
       </c>
       <c r="B139" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="140">
@@ -1895,7 +1895,7 @@
         <v>72</v>
       </c>
       <c r="B152" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="153">
@@ -2063,7 +2063,7 @@
         <v>72</v>
       </c>
       <c r="B173" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="174">
@@ -2071,7 +2071,7 @@
         <v>72</v>
       </c>
       <c r="B174" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
     </row>
     <row r="175">
@@ -2079,7 +2079,7 @@
         <v>72</v>
       </c>
       <c r="B175" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
     <row r="176">
@@ -2087,7 +2087,7 @@
         <v>72</v>
       </c>
       <c r="B176" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
     </row>
     <row r="177">
@@ -2095,7 +2095,7 @@
         <v>72</v>
       </c>
       <c r="B177" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="178">
@@ -2103,7 +2103,7 @@
         <v>72</v>
       </c>
       <c r="B178" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
     </row>
     <row r="179">
@@ -2111,7 +2111,7 @@
         <v>72</v>
       </c>
       <c r="B179" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="180">
@@ -2319,7 +2319,7 @@
         <v>94</v>
       </c>
       <c r="B205" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="206">
@@ -2479,7 +2479,7 @@
         <v>94</v>
       </c>
       <c r="B225" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="226">
@@ -2695,7 +2695,7 @@
         <v>94</v>
       </c>
       <c r="B252" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="253">
@@ -2791,7 +2791,7 @@
         <v>106</v>
       </c>
       <c r="B264" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="265">
@@ -2855,7 +2855,7 @@
         <v>106</v>
       </c>
       <c r="B272" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="273">
@@ -2943,7 +2943,7 @@
         <v>106</v>
       </c>
       <c r="B283" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="284">
@@ -3039,7 +3039,7 @@
         <v>106</v>
       </c>
       <c r="B295" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="296">

</xml_diff>

<commit_message>
added sorting by ascending order per year
</commit_message>
<xml_diff>
--- a/data/01 application country names per year.xlsx
+++ b/data/01 application country names per year.xlsx
@@ -23,334 +23,334 @@
     <t>2011</t>
   </si>
   <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Congo, the Democratic Republic of the</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
     <t>India</t>
   </si>
   <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Korea, Republic of</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Lao People's Democratic Republic</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Palestine, State of</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
     <t>Tanzania, United Republic of</t>
   </si>
   <si>
-    <t>Indonesia</t>
-  </si>
-  <si>
-    <t>Nigeria</t>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Timor-Leste</t>
+  </si>
+  <si>
+    <t>Uganda</t>
   </si>
   <si>
     <t>United States</t>
   </si>
   <si>
+    <t>Viet Nam</t>
+  </si>
+  <si>
     <t>Zambia</t>
   </si>
   <si>
-    <t>Mauritius</t>
-  </si>
-  <si>
-    <t>South Africa</t>
-  </si>
-  <si>
-    <t>Ghana</t>
-  </si>
-  <si>
-    <t>Kenya</t>
-  </si>
-  <si>
-    <t>Congo, the Democratic Republic of the</t>
-  </si>
-  <si>
-    <t>Viet Nam</t>
-  </si>
-  <si>
-    <t>Nepal</t>
-  </si>
-  <si>
-    <t>Rwanda</t>
-  </si>
-  <si>
-    <t>Cameroon</t>
-  </si>
-  <si>
-    <t>Lesotho</t>
-  </si>
-  <si>
-    <t>Israel</t>
-  </si>
-  <si>
-    <t>Uganda</t>
-  </si>
-  <si>
-    <t>Egypt</t>
-  </si>
-  <si>
-    <t>Ethiopia</t>
-  </si>
-  <si>
-    <t>Cambodia</t>
-  </si>
-  <si>
-    <t>Singapore</t>
-  </si>
-  <si>
-    <t>Pakistan</t>
-  </si>
-  <si>
-    <t>Philippines</t>
-  </si>
-  <si>
-    <t>Palestine, State of</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Malawi</t>
-  </si>
-  <si>
-    <t>Iraq</t>
-  </si>
-  <si>
-    <t>Afghanistan</t>
-  </si>
-  <si>
     <t>Zimbabwe</t>
   </si>
   <si>
-    <t>Korea, Republic of</t>
-  </si>
-  <si>
-    <t>Mali</t>
-  </si>
-  <si>
-    <t>Bangladesh</t>
-  </si>
-  <si>
-    <t>Bhutan</t>
-  </si>
-  <si>
-    <t>Timor-Leste</t>
-  </si>
-  <si>
-    <t>Lao People's Democratic Republic</t>
-  </si>
-  <si>
-    <t>Thailand</t>
-  </si>
-  <si>
-    <t>Morocco</t>
-  </si>
-  <si>
-    <t>Malaysia</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>Sri Lanka</t>
-  </si>
-  <si>
-    <t>Liberia</t>
-  </si>
-  <si>
-    <t>Central African Republic</t>
-  </si>
-  <si>
-    <t>Mauritania</t>
-  </si>
-  <si>
-    <t>Burundi</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>Kyrgyzstan</t>
-  </si>
-  <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>Lebanon</t>
-  </si>
-  <si>
-    <t>Sierra Leone</t>
-  </si>
-  <si>
-    <t>Somalia</t>
-  </si>
-  <si>
     <t>2012</t>
   </si>
   <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>Iran, Islamic Republic of</t>
+  </si>
+  <si>
+    <t>Korea, Democratic People's Republic of</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Papua New Guinea</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Solomon Islands</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
     <t>Tunisia</t>
   </si>
   <si>
-    <t>Papua New Guinea</t>
-  </si>
-  <si>
-    <t>Sudan</t>
-  </si>
-  <si>
-    <t>Senegal</t>
+    <t>United Kingdom</t>
   </si>
   <si>
     <t>Yemen</t>
   </si>
   <si>
-    <t>Namibia</t>
-  </si>
-  <si>
-    <t>Mozambique</t>
-  </si>
-  <si>
-    <t>Solomon Islands</t>
-  </si>
-  <si>
-    <t>Botswana</t>
-  </si>
-  <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>Iran, Islamic Republic of</t>
-  </si>
-  <si>
-    <t>Madagascar</t>
-  </si>
-  <si>
-    <t>Korea, Democratic People's Republic of</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
     <t>2013</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>Bolivia, Plurinational State of</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>Côte d'Ivoire</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Maldives</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
     <t>Niger</t>
   </si>
   <si>
-    <t>Congo</t>
-  </si>
-  <si>
     <t>Portugal</t>
   </si>
   <si>
-    <t>Chad</t>
-  </si>
-  <si>
     <t>Slovenia</t>
   </si>
   <si>
-    <t>Jordan</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Maldives</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>New Zealand</t>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Swaziland</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
   </si>
   <si>
     <t>Togo</t>
   </si>
   <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>Côte d'Ivoire</t>
-  </si>
-  <si>
-    <t>Tajikistan</t>
-  </si>
-  <si>
-    <t>Burkina Faso</t>
-  </si>
-  <si>
-    <t>Gambia</t>
-  </si>
-  <si>
-    <t>Iceland</t>
-  </si>
-  <si>
-    <t>Bolivia, Plurinational State of</t>
-  </si>
-  <si>
-    <t>Finland</t>
-  </si>
-  <si>
-    <t>Swaziland</t>
-  </si>
-  <si>
     <t>2014</t>
   </si>
   <si>
+    <t>American Samoa</t>
+  </si>
+  <si>
     <t>Armenia</t>
   </si>
   <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
     <t>Benin</t>
   </si>
   <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
     <t>Romania</t>
   </si>
   <si>
     <t>Syrian Arab Republic</t>
   </si>
   <si>
-    <t>Kazakhstan</t>
-  </si>
-  <si>
-    <t>Costa Rica</t>
-  </si>
-  <si>
-    <t>Guinea</t>
-  </si>
-  <si>
-    <t>Bahrain</t>
+    <t>Turkey</t>
   </si>
   <si>
     <t>Ukraine</t>
   </si>
   <si>
-    <t>American Samoa</t>
-  </si>
-  <si>
-    <t>Turkey</t>
-  </si>
-  <si>
     <t>2015</t>
   </si>
   <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
     <t>Mongolia</t>
   </si>
   <si>
     <t>Myanmar</t>
   </si>
   <si>
-    <t>Austria</t>
-  </si>
-  <si>
-    <t>Colombia</t>
-  </si>
-  <si>
     <t>Serbia</t>
-  </si>
-  <si>
-    <t>Bulgaria</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1127,7 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
@@ -1135,7 +1135,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58">
@@ -1143,7 +1143,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59">
@@ -1151,7 +1151,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60">
@@ -1167,7 +1167,7 @@
         <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62">
@@ -1175,7 +1175,7 @@
         <v>57</v>
       </c>
       <c r="B62" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63">
@@ -1183,7 +1183,7 @@
         <v>57</v>
       </c>
       <c r="B63" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64">
@@ -1191,7 +1191,7 @@
         <v>57</v>
       </c>
       <c r="B64" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65">
@@ -1199,7 +1199,7 @@
         <v>57</v>
       </c>
       <c r="B65" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66">
@@ -1207,7 +1207,7 @@
         <v>57</v>
       </c>
       <c r="B66" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67">
@@ -1215,7 +1215,7 @@
         <v>57</v>
       </c>
       <c r="B67" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68">
@@ -1223,7 +1223,7 @@
         <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69">
@@ -1231,7 +1231,7 @@
         <v>57</v>
       </c>
       <c r="B69" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70">
@@ -1239,7 +1239,7 @@
         <v>57</v>
       </c>
       <c r="B70" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71">
@@ -1247,7 +1247,7 @@
         <v>57</v>
       </c>
       <c r="B71" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72">
@@ -1255,7 +1255,7 @@
         <v>57</v>
       </c>
       <c r="B72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73">
@@ -1263,7 +1263,7 @@
         <v>57</v>
       </c>
       <c r="B73" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row r="74">
@@ -1271,7 +1271,7 @@
         <v>57</v>
       </c>
       <c r="B74" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="75">
@@ -1279,7 +1279,7 @@
         <v>57</v>
       </c>
       <c r="B75" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
     </row>
     <row r="76">
@@ -1287,7 +1287,7 @@
         <v>57</v>
       </c>
       <c r="B76" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="77">
@@ -1295,7 +1295,7 @@
         <v>57</v>
       </c>
       <c r="B77" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="78">
@@ -1303,7 +1303,7 @@
         <v>57</v>
       </c>
       <c r="B78" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79">
@@ -1311,7 +1311,7 @@
         <v>57</v>
       </c>
       <c r="B79" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="80">
@@ -1319,7 +1319,7 @@
         <v>57</v>
       </c>
       <c r="B80" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="81">
@@ -1327,7 +1327,7 @@
         <v>57</v>
       </c>
       <c r="B81" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
     </row>
     <row r="82">
@@ -1335,7 +1335,7 @@
         <v>57</v>
       </c>
       <c r="B82" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
     <row r="83">
@@ -1343,7 +1343,7 @@
         <v>57</v>
       </c>
       <c r="B83" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="84">
@@ -1351,7 +1351,7 @@
         <v>57</v>
       </c>
       <c r="B84" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85">
@@ -1359,7 +1359,7 @@
         <v>57</v>
       </c>
       <c r="B85" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86">
@@ -1367,7 +1367,7 @@
         <v>57</v>
       </c>
       <c r="B86" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="87">
@@ -1375,7 +1375,7 @@
         <v>57</v>
       </c>
       <c r="B87" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="88">
@@ -1383,7 +1383,7 @@
         <v>57</v>
       </c>
       <c r="B88" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="89">
@@ -1391,7 +1391,7 @@
         <v>57</v>
       </c>
       <c r="B89" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="90">
@@ -1399,7 +1399,7 @@
         <v>57</v>
       </c>
       <c r="B90" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
     </row>
     <row r="91">
@@ -1407,7 +1407,7 @@
         <v>57</v>
       </c>
       <c r="B91" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
     </row>
     <row r="92">
@@ -1415,7 +1415,7 @@
         <v>57</v>
       </c>
       <c r="B92" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="93">
@@ -1423,7 +1423,7 @@
         <v>57</v>
       </c>
       <c r="B93" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="94">
@@ -1431,7 +1431,7 @@
         <v>57</v>
       </c>
       <c r="B94" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
     </row>
     <row r="95">
@@ -1439,7 +1439,7 @@
         <v>57</v>
       </c>
       <c r="B95" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
     </row>
     <row r="96">
@@ -1447,7 +1447,7 @@
         <v>57</v>
       </c>
       <c r="B96" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="97">
@@ -1455,7 +1455,7 @@
         <v>57</v>
       </c>
       <c r="B97" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
     </row>
     <row r="98">
@@ -1463,7 +1463,7 @@
         <v>57</v>
       </c>
       <c r="B98" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="99">
@@ -1471,7 +1471,7 @@
         <v>57</v>
       </c>
       <c r="B99" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="100">
@@ -1479,7 +1479,7 @@
         <v>57</v>
       </c>
       <c r="B100" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="101">
@@ -1487,7 +1487,7 @@
         <v>57</v>
       </c>
       <c r="B101" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
     </row>
     <row r="102">
@@ -1495,7 +1495,7 @@
         <v>57</v>
       </c>
       <c r="B102" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="103">
@@ -1503,7 +1503,7 @@
         <v>57</v>
       </c>
       <c r="B103" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="104">
@@ -1511,7 +1511,7 @@
         <v>57</v>
       </c>
       <c r="B104" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="105">
@@ -1519,7 +1519,7 @@
         <v>57</v>
       </c>
       <c r="B105" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="106">
@@ -1527,7 +1527,7 @@
         <v>57</v>
       </c>
       <c r="B106" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="107">
@@ -1535,7 +1535,7 @@
         <v>57</v>
       </c>
       <c r="B107" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
     </row>
     <row r="108">
@@ -1543,7 +1543,7 @@
         <v>57</v>
       </c>
       <c r="B108" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="109">
@@ -1551,7 +1551,7 @@
         <v>57</v>
       </c>
       <c r="B109" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="110">
@@ -1559,7 +1559,7 @@
         <v>57</v>
       </c>
       <c r="B110" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="111">
@@ -1567,7 +1567,7 @@
         <v>57</v>
       </c>
       <c r="B111" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="112">
@@ -1575,7 +1575,7 @@
         <v>72</v>
       </c>
       <c r="B112" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
     </row>
     <row r="113">
@@ -1583,7 +1583,7 @@
         <v>72</v>
       </c>
       <c r="B113" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114">
@@ -1591,7 +1591,7 @@
         <v>72</v>
       </c>
       <c r="B114" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115">
@@ -1599,7 +1599,7 @@
         <v>72</v>
       </c>
       <c r="B115" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116">
@@ -1607,7 +1607,7 @@
         <v>72</v>
       </c>
       <c r="B116" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="117">
@@ -1615,7 +1615,7 @@
         <v>72</v>
       </c>
       <c r="B117" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
     </row>
     <row r="118">
@@ -1623,7 +1623,7 @@
         <v>72</v>
       </c>
       <c r="B118" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
     </row>
     <row r="119">
@@ -1631,7 +1631,7 @@
         <v>72</v>
       </c>
       <c r="B119" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120">
@@ -1639,7 +1639,7 @@
         <v>72</v>
       </c>
       <c r="B120" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
     </row>
     <row r="121">
@@ -1647,7 +1647,7 @@
         <v>72</v>
       </c>
       <c r="B121" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122">
@@ -1655,7 +1655,7 @@
         <v>72</v>
       </c>
       <c r="B122" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="123">
@@ -1663,7 +1663,7 @@
         <v>72</v>
       </c>
       <c r="B123" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
     </row>
     <row r="124">
@@ -1671,7 +1671,7 @@
         <v>72</v>
       </c>
       <c r="B124" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
     </row>
     <row r="125">
@@ -1679,7 +1679,7 @@
         <v>72</v>
       </c>
       <c r="B125" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="126">
@@ -1687,7 +1687,7 @@
         <v>72</v>
       </c>
       <c r="B126" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
     </row>
     <row r="127">
@@ -1695,7 +1695,7 @@
         <v>72</v>
       </c>
       <c r="B127" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="128">
@@ -1703,7 +1703,7 @@
         <v>72</v>
       </c>
       <c r="B128" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="129">
@@ -1711,7 +1711,7 @@
         <v>72</v>
       </c>
       <c r="B129" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
     </row>
     <row r="130">
@@ -1719,7 +1719,7 @@
         <v>72</v>
       </c>
       <c r="B130" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
     </row>
     <row r="131">
@@ -1727,7 +1727,7 @@
         <v>72</v>
       </c>
       <c r="B131" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
     </row>
     <row r="132">
@@ -1735,7 +1735,7 @@
         <v>72</v>
       </c>
       <c r="B132" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
     </row>
     <row r="133">
@@ -1743,7 +1743,7 @@
         <v>72</v>
       </c>
       <c r="B133" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="134">
@@ -1751,7 +1751,7 @@
         <v>72</v>
       </c>
       <c r="B134" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="135">
@@ -1759,7 +1759,7 @@
         <v>72</v>
       </c>
       <c r="B135" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
     </row>
     <row r="136">
@@ -1767,7 +1767,7 @@
         <v>72</v>
       </c>
       <c r="B136" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
     </row>
     <row r="137">
@@ -1775,7 +1775,7 @@
         <v>72</v>
       </c>
       <c r="B137" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="138">
@@ -1783,7 +1783,7 @@
         <v>72</v>
       </c>
       <c r="B138" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
     </row>
     <row r="139">
@@ -1791,7 +1791,7 @@
         <v>72</v>
       </c>
       <c r="B139" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
     </row>
     <row r="140">
@@ -1799,7 +1799,7 @@
         <v>72</v>
       </c>
       <c r="B140" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="141">
@@ -1807,7 +1807,7 @@
         <v>72</v>
       </c>
       <c r="B141" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="142">
@@ -1815,7 +1815,7 @@
         <v>72</v>
       </c>
       <c r="B142" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
     </row>
     <row r="143">
@@ -1823,7 +1823,7 @@
         <v>72</v>
       </c>
       <c r="B143" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
     </row>
     <row r="144">
@@ -1831,7 +1831,7 @@
         <v>72</v>
       </c>
       <c r="B144" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="145">
@@ -1839,7 +1839,7 @@
         <v>72</v>
       </c>
       <c r="B145" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="146">
@@ -1847,7 +1847,7 @@
         <v>72</v>
       </c>
       <c r="B146" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
     </row>
     <row r="147">
@@ -1855,7 +1855,7 @@
         <v>72</v>
       </c>
       <c r="B147" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
     </row>
     <row r="148">
@@ -1863,7 +1863,7 @@
         <v>72</v>
       </c>
       <c r="B148" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="149">
@@ -1871,7 +1871,7 @@
         <v>72</v>
       </c>
       <c r="B149" t="s">
-        <v>79</v>
+        <v>36</v>
       </c>
     </row>
     <row r="150">
@@ -1879,7 +1879,7 @@
         <v>72</v>
       </c>
       <c r="B150" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="151">
@@ -1887,7 +1887,7 @@
         <v>72</v>
       </c>
       <c r="B151" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="152">
@@ -1895,7 +1895,7 @@
         <v>72</v>
       </c>
       <c r="B152" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
     </row>
     <row r="153">
@@ -1903,7 +1903,7 @@
         <v>72</v>
       </c>
       <c r="B153" t="s">
-        <v>5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="154">
@@ -1911,7 +1911,7 @@
         <v>72</v>
       </c>
       <c r="B154" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
     </row>
     <row r="155">
@@ -1919,7 +1919,7 @@
         <v>72</v>
       </c>
       <c r="B155" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
     </row>
     <row r="156">
@@ -1927,7 +1927,7 @@
         <v>72</v>
       </c>
       <c r="B156" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="157">
@@ -1935,7 +1935,7 @@
         <v>72</v>
       </c>
       <c r="B157" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="158">
@@ -1943,7 +1943,7 @@
         <v>72</v>
       </c>
       <c r="B158" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
     </row>
     <row r="159">
@@ -1951,7 +1951,7 @@
         <v>72</v>
       </c>
       <c r="B159" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
     </row>
     <row r="160">
@@ -1959,7 +1959,7 @@
         <v>72</v>
       </c>
       <c r="B160" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
     <row r="161">
@@ -1967,7 +1967,7 @@
         <v>72</v>
       </c>
       <c r="B161" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
     </row>
     <row r="162">
@@ -1975,7 +1975,7 @@
         <v>72</v>
       </c>
       <c r="B162" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="163">
@@ -1983,7 +1983,7 @@
         <v>72</v>
       </c>
       <c r="B163" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="164">
@@ -1991,7 +1991,7 @@
         <v>72</v>
       </c>
       <c r="B164" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
     </row>
     <row r="165">
@@ -1999,7 +1999,7 @@
         <v>72</v>
       </c>
       <c r="B165" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
     </row>
     <row r="166">
@@ -2007,7 +2007,7 @@
         <v>72</v>
       </c>
       <c r="B166" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="167">
@@ -2015,7 +2015,7 @@
         <v>72</v>
       </c>
       <c r="B167" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="168">
@@ -2023,7 +2023,7 @@
         <v>72</v>
       </c>
       <c r="B168" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="169">
@@ -2031,7 +2031,7 @@
         <v>72</v>
       </c>
       <c r="B169" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
     </row>
     <row r="170">
@@ -2039,7 +2039,7 @@
         <v>72</v>
       </c>
       <c r="B170" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="171">
@@ -2047,7 +2047,7 @@
         <v>72</v>
       </c>
       <c r="B171" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
     </row>
     <row r="172">
@@ -2055,7 +2055,7 @@
         <v>72</v>
       </c>
       <c r="B172" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
     </row>
     <row r="173">
@@ -2063,7 +2063,7 @@
         <v>72</v>
       </c>
       <c r="B173" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
     </row>
     <row r="174">
@@ -2071,7 +2071,7 @@
         <v>72</v>
       </c>
       <c r="B174" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
     </row>
     <row r="175">
@@ -2079,7 +2079,7 @@
         <v>72</v>
       </c>
       <c r="B175" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="176">
@@ -2087,7 +2087,7 @@
         <v>72</v>
       </c>
       <c r="B176" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="177">
@@ -2095,7 +2095,7 @@
         <v>72</v>
       </c>
       <c r="B177" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="178">
@@ -2103,7 +2103,7 @@
         <v>72</v>
       </c>
       <c r="B178" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="179">
@@ -2111,7 +2111,7 @@
         <v>72</v>
       </c>
       <c r="B179" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="180">
@@ -2119,7 +2119,7 @@
         <v>72</v>
       </c>
       <c r="B180" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
     </row>
     <row r="181">
@@ -2127,7 +2127,7 @@
         <v>72</v>
       </c>
       <c r="B181" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
     </row>
     <row r="182">
@@ -2135,7 +2135,7 @@
         <v>72</v>
       </c>
       <c r="B182" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
     </row>
     <row r="183">
@@ -2143,7 +2143,7 @@
         <v>72</v>
       </c>
       <c r="B183" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
     </row>
     <row r="184">
@@ -2151,7 +2151,7 @@
         <v>72</v>
       </c>
       <c r="B184" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
     </row>
     <row r="185">
@@ -2159,7 +2159,7 @@
         <v>72</v>
       </c>
       <c r="B185" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
     </row>
     <row r="186">
@@ -2167,7 +2167,7 @@
         <v>94</v>
       </c>
       <c r="B186" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="187">
@@ -2175,7 +2175,7 @@
         <v>94</v>
       </c>
       <c r="B187" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="188">
@@ -2183,7 +2183,7 @@
         <v>94</v>
       </c>
       <c r="B188" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
     </row>
     <row r="189">
@@ -2191,7 +2191,7 @@
         <v>94</v>
       </c>
       <c r="B189" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="190">
@@ -2199,7 +2199,7 @@
         <v>94</v>
       </c>
       <c r="B190" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
     </row>
     <row r="191">
@@ -2207,7 +2207,7 @@
         <v>94</v>
       </c>
       <c r="B191" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="192">
@@ -2215,7 +2215,7 @@
         <v>94</v>
       </c>
       <c r="B192" t="s">
-        <v>3</v>
+        <v>98</v>
       </c>
     </row>
     <row r="193">
@@ -2223,7 +2223,7 @@
         <v>94</v>
       </c>
       <c r="B193" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="194">
@@ -2231,7 +2231,7 @@
         <v>94</v>
       </c>
       <c r="B194" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="195">
@@ -2239,7 +2239,7 @@
         <v>94</v>
       </c>
       <c r="B195" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="196">
@@ -2255,7 +2255,7 @@
         <v>94</v>
       </c>
       <c r="B197" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198">
@@ -2263,7 +2263,7 @@
         <v>94</v>
       </c>
       <c r="B198" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="199">
@@ -2271,7 +2271,7 @@
         <v>94</v>
       </c>
       <c r="B199" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
     </row>
     <row r="200">
@@ -2279,7 +2279,7 @@
         <v>94</v>
       </c>
       <c r="B200" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
     </row>
     <row r="201">
@@ -2287,7 +2287,7 @@
         <v>94</v>
       </c>
       <c r="B201" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="202">
@@ -2295,7 +2295,7 @@
         <v>94</v>
       </c>
       <c r="B202" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="203">
@@ -2303,7 +2303,7 @@
         <v>94</v>
       </c>
       <c r="B203" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
     </row>
     <row r="204">
@@ -2311,7 +2311,7 @@
         <v>94</v>
       </c>
       <c r="B204" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
     </row>
     <row r="205">
@@ -2319,7 +2319,7 @@
         <v>94</v>
       </c>
       <c r="B205" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
     </row>
     <row r="206">
@@ -2327,7 +2327,7 @@
         <v>94</v>
       </c>
       <c r="B206" t="s">
-        <v>95</v>
+        <v>19</v>
       </c>
     </row>
     <row r="207">
@@ -2335,7 +2335,7 @@
         <v>94</v>
       </c>
       <c r="B207" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
     </row>
     <row r="208">
@@ -2343,7 +2343,7 @@
         <v>94</v>
       </c>
       <c r="B208" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
     </row>
     <row r="209">
@@ -2351,7 +2351,7 @@
         <v>94</v>
       </c>
       <c r="B209" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="210">
@@ -2359,7 +2359,7 @@
         <v>94</v>
       </c>
       <c r="B210" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="211">
@@ -2367,7 +2367,7 @@
         <v>94</v>
       </c>
       <c r="B211" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
     </row>
     <row r="212">
@@ -2375,7 +2375,7 @@
         <v>94</v>
       </c>
       <c r="B212" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
     </row>
     <row r="213">
@@ -2383,7 +2383,7 @@
         <v>94</v>
       </c>
       <c r="B213" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
     </row>
     <row r="214">
@@ -2391,7 +2391,7 @@
         <v>94</v>
       </c>
       <c r="B214" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="215">
@@ -2399,7 +2399,7 @@
         <v>94</v>
       </c>
       <c r="B215" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
     </row>
     <row r="216">
@@ -2407,7 +2407,7 @@
         <v>94</v>
       </c>
       <c r="B216" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="217">
@@ -2415,7 +2415,7 @@
         <v>94</v>
       </c>
       <c r="B217" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
     </row>
     <row r="218">
@@ -2423,7 +2423,7 @@
         <v>94</v>
       </c>
       <c r="B218" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="219">
@@ -2431,7 +2431,7 @@
         <v>94</v>
       </c>
       <c r="B219" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="220">
@@ -2439,7 +2439,7 @@
         <v>94</v>
       </c>
       <c r="B220" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="221">
@@ -2447,7 +2447,7 @@
         <v>94</v>
       </c>
       <c r="B221" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
     </row>
     <row r="222">
@@ -2455,7 +2455,7 @@
         <v>94</v>
       </c>
       <c r="B222" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="223">
@@ -2463,7 +2463,7 @@
         <v>94</v>
       </c>
       <c r="B223" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
     </row>
     <row r="224">
@@ -2471,7 +2471,7 @@
         <v>94</v>
       </c>
       <c r="B224" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="225">
@@ -2479,7 +2479,7 @@
         <v>94</v>
       </c>
       <c r="B225" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
     </row>
     <row r="226">
@@ -2487,7 +2487,7 @@
         <v>94</v>
       </c>
       <c r="B226" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="227">
@@ -2495,7 +2495,7 @@
         <v>94</v>
       </c>
       <c r="B227" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="228">
@@ -2503,7 +2503,7 @@
         <v>94</v>
       </c>
       <c r="B228" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
     </row>
     <row r="229">
@@ -2511,7 +2511,7 @@
         <v>94</v>
       </c>
       <c r="B229" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="230">
@@ -2519,7 +2519,7 @@
         <v>94</v>
       </c>
       <c r="B230" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="231">
@@ -2527,7 +2527,7 @@
         <v>94</v>
       </c>
       <c r="B231" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="232">
@@ -2535,7 +2535,7 @@
         <v>94</v>
       </c>
       <c r="B232" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="233">
@@ -2543,7 +2543,7 @@
         <v>94</v>
       </c>
       <c r="B233" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
     </row>
     <row r="234">
@@ -2551,7 +2551,7 @@
         <v>94</v>
       </c>
       <c r="B234" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="235">
@@ -2559,7 +2559,7 @@
         <v>94</v>
       </c>
       <c r="B235" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="236">
@@ -2567,7 +2567,7 @@
         <v>94</v>
       </c>
       <c r="B236" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
     </row>
     <row r="237">
@@ -2575,7 +2575,7 @@
         <v>94</v>
       </c>
       <c r="B237" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="238">
@@ -2583,7 +2583,7 @@
         <v>94</v>
       </c>
       <c r="B238" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
     </row>
     <row r="239">
@@ -2591,7 +2591,7 @@
         <v>94</v>
       </c>
       <c r="B239" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
     </row>
     <row r="240">
@@ -2599,7 +2599,7 @@
         <v>94</v>
       </c>
       <c r="B240" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
     </row>
     <row r="241">
@@ -2607,7 +2607,7 @@
         <v>94</v>
       </c>
       <c r="B241" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
     </row>
     <row r="242">
@@ -2615,7 +2615,7 @@
         <v>94</v>
       </c>
       <c r="B242" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="243">
@@ -2623,7 +2623,7 @@
         <v>94</v>
       </c>
       <c r="B243" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="244">
@@ -2631,7 +2631,7 @@
         <v>94</v>
       </c>
       <c r="B244" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
     </row>
     <row r="245">
@@ -2639,7 +2639,7 @@
         <v>94</v>
       </c>
       <c r="B245" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
     </row>
     <row r="246">
@@ -2647,7 +2647,7 @@
         <v>94</v>
       </c>
       <c r="B246" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="247">
@@ -2655,7 +2655,7 @@
         <v>94</v>
       </c>
       <c r="B247" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
     </row>
     <row r="248">
@@ -2663,7 +2663,7 @@
         <v>94</v>
       </c>
       <c r="B248" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="249">
@@ -2671,7 +2671,7 @@
         <v>94</v>
       </c>
       <c r="B249" t="s">
-        <v>104</v>
+        <v>54</v>
       </c>
     </row>
     <row r="250">
@@ -2679,7 +2679,7 @@
         <v>94</v>
       </c>
       <c r="B250" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
     </row>
     <row r="251">
@@ -2687,7 +2687,7 @@
         <v>94</v>
       </c>
       <c r="B251" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="252">
@@ -2695,7 +2695,7 @@
         <v>94</v>
       </c>
       <c r="B252" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="253">
@@ -2703,7 +2703,7 @@
         <v>106</v>
       </c>
       <c r="B253" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="254">
@@ -2711,7 +2711,7 @@
         <v>106</v>
       </c>
       <c r="B254" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="255">
@@ -2719,7 +2719,7 @@
         <v>106</v>
       </c>
       <c r="B255" t="s">
-        <v>40</v>
+        <v>107</v>
       </c>
     </row>
     <row r="256">
@@ -2727,7 +2727,7 @@
         <v>106</v>
       </c>
       <c r="B256" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="257">
@@ -2735,7 +2735,7 @@
         <v>106</v>
       </c>
       <c r="B257" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="258">
@@ -2743,7 +2743,7 @@
         <v>106</v>
       </c>
       <c r="B258" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="259">
@@ -2751,7 +2751,7 @@
         <v>106</v>
       </c>
       <c r="B259" t="s">
-        <v>11</v>
+        <v>108</v>
       </c>
     </row>
     <row r="260">
@@ -2759,7 +2759,7 @@
         <v>106</v>
       </c>
       <c r="B260" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
     </row>
     <row r="261">
@@ -2767,7 +2767,7 @@
         <v>106</v>
       </c>
       <c r="B261" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="262">
@@ -2775,7 +2775,7 @@
         <v>106</v>
       </c>
       <c r="B262" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="263">
@@ -2783,7 +2783,7 @@
         <v>106</v>
       </c>
       <c r="B263" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
     </row>
     <row r="264">
@@ -2791,7 +2791,7 @@
         <v>106</v>
       </c>
       <c r="B264" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
     </row>
     <row r="265">
@@ -2799,7 +2799,7 @@
         <v>106</v>
       </c>
       <c r="B265" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
     </row>
     <row r="266">
@@ -2807,7 +2807,7 @@
         <v>106</v>
       </c>
       <c r="B266" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="267">
@@ -2815,7 +2815,7 @@
         <v>106</v>
       </c>
       <c r="B267" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="268">
@@ -2823,7 +2823,7 @@
         <v>106</v>
       </c>
       <c r="B268" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="269">
@@ -2831,7 +2831,7 @@
         <v>106</v>
       </c>
       <c r="B269" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
     </row>
     <row r="270">
@@ -2839,7 +2839,7 @@
         <v>106</v>
       </c>
       <c r="B270" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="271">
@@ -2847,7 +2847,7 @@
         <v>106</v>
       </c>
       <c r="B271" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="272">
@@ -2855,7 +2855,7 @@
         <v>106</v>
       </c>
       <c r="B272" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="273">
@@ -2863,7 +2863,7 @@
         <v>106</v>
       </c>
       <c r="B273" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="274">
@@ -2871,7 +2871,7 @@
         <v>106</v>
       </c>
       <c r="B274" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="275">
@@ -2879,7 +2879,7 @@
         <v>106</v>
       </c>
       <c r="B275" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="276">
@@ -2887,7 +2887,7 @@
         <v>106</v>
       </c>
       <c r="B276" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
     </row>
     <row r="277">
@@ -2895,7 +2895,7 @@
         <v>106</v>
       </c>
       <c r="B277" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="278">
@@ -2903,7 +2903,7 @@
         <v>106</v>
       </c>
       <c r="B278" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="279">
@@ -2911,7 +2911,7 @@
         <v>106</v>
       </c>
       <c r="B279" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="280">
@@ -2919,7 +2919,7 @@
         <v>106</v>
       </c>
       <c r="B280" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
     </row>
     <row r="281">
@@ -2927,7 +2927,7 @@
         <v>106</v>
       </c>
       <c r="B281" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
     </row>
     <row r="282">
@@ -2935,7 +2935,7 @@
         <v>106</v>
       </c>
       <c r="B282" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="283">
@@ -2943,7 +2943,7 @@
         <v>106</v>
       </c>
       <c r="B283" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="284">
@@ -2951,7 +2951,7 @@
         <v>106</v>
       </c>
       <c r="B284" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
     </row>
     <row r="285">
@@ -2959,7 +2959,7 @@
         <v>106</v>
       </c>
       <c r="B285" t="s">
-        <v>108</v>
+        <v>63</v>
       </c>
     </row>
     <row r="286">
@@ -2967,7 +2967,7 @@
         <v>106</v>
       </c>
       <c r="B286" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="287">
@@ -2975,7 +2975,7 @@
         <v>106</v>
       </c>
       <c r="B287" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
     </row>
     <row r="288">
@@ -2983,7 +2983,7 @@
         <v>106</v>
       </c>
       <c r="B288" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
     </row>
     <row r="289">
@@ -2991,7 +2991,7 @@
         <v>106</v>
       </c>
       <c r="B289" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
     </row>
     <row r="290">
@@ -2999,7 +2999,7 @@
         <v>106</v>
       </c>
       <c r="B290" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="291">
@@ -3007,7 +3007,7 @@
         <v>106</v>
       </c>
       <c r="B291" t="s">
-        <v>101</v>
+        <v>42</v>
       </c>
     </row>
     <row r="292">
@@ -3015,7 +3015,7 @@
         <v>106</v>
       </c>
       <c r="B292" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
     </row>
     <row r="293">
@@ -3023,7 +3023,7 @@
         <v>106</v>
       </c>
       <c r="B293" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="294">
@@ -3031,7 +3031,7 @@
         <v>106</v>
       </c>
       <c r="B294" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
     </row>
     <row r="295">
@@ -3039,7 +3039,7 @@
         <v>106</v>
       </c>
       <c r="B295" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="296">
@@ -3047,7 +3047,7 @@
         <v>106</v>
       </c>
       <c r="B296" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="297">
@@ -3055,7 +3055,7 @@
         <v>106</v>
       </c>
       <c r="B297" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="298">
@@ -3063,7 +3063,7 @@
         <v>106</v>
       </c>
       <c r="B298" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="299">
@@ -3071,7 +3071,7 @@
         <v>106</v>
       </c>
       <c r="B299" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="300">
@@ -3079,7 +3079,7 @@
         <v>106</v>
       </c>
       <c r="B300" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="301">
@@ -3087,7 +3087,7 @@
         <v>106</v>
       </c>
       <c r="B301" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="302">
@@ -3095,7 +3095,7 @@
         <v>106</v>
       </c>
       <c r="B302" t="s">
-        <v>111</v>
+        <v>52</v>
       </c>
     </row>
     <row r="303">
@@ -3103,7 +3103,7 @@
         <v>106</v>
       </c>
       <c r="B303" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="304">
@@ -3111,7 +3111,7 @@
         <v>106</v>
       </c>
       <c r="B304" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
     </row>
     <row r="305">
@@ -3119,7 +3119,7 @@
         <v>106</v>
       </c>
       <c r="B305" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
     </row>
     <row r="306">
@@ -3127,7 +3127,7 @@
         <v>106</v>
       </c>
       <c r="B306" t="s">
-        <v>112</v>
+        <v>55</v>
       </c>
     </row>
     <row r="307">

</xml_diff>

<commit_message>
process applied and impact countries to count separately
</commit_message>
<xml_diff>
--- a/data/01 application country names per year.xlsx
+++ b/data/01 application country names per year.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>project_year</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t>2013</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Bolivia, Plurinational State of</t>
@@ -1575,7 +1572,7 @@
         <v>72</v>
       </c>
       <c r="B112" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113">
@@ -1583,7 +1580,7 @@
         <v>72</v>
       </c>
       <c r="B113" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114">
@@ -1591,7 +1588,7 @@
         <v>72</v>
       </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115">
@@ -1599,7 +1596,7 @@
         <v>72</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
     </row>
     <row r="116">
@@ -1607,7 +1604,7 @@
         <v>72</v>
       </c>
       <c r="B116" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
     <row r="117">
@@ -1615,7 +1612,7 @@
         <v>72</v>
       </c>
       <c r="B117" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
     </row>
     <row r="118">
@@ -1623,7 +1620,7 @@
         <v>72</v>
       </c>
       <c r="B118" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
     </row>
     <row r="119">
@@ -1631,7 +1628,7 @@
         <v>72</v>
       </c>
       <c r="B119" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120">
@@ -1639,7 +1636,7 @@
         <v>72</v>
       </c>
       <c r="B120" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121">
@@ -1647,7 +1644,7 @@
         <v>72</v>
       </c>
       <c r="B121" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="122">
@@ -1655,7 +1652,7 @@
         <v>72</v>
       </c>
       <c r="B122" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
     </row>
     <row r="123">
@@ -1671,7 +1668,7 @@
         <v>72</v>
       </c>
       <c r="B124" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
     </row>
     <row r="125">
@@ -1679,7 +1676,7 @@
         <v>72</v>
       </c>
       <c r="B125" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
     </row>
     <row r="126">
@@ -1687,7 +1684,7 @@
         <v>72</v>
       </c>
       <c r="B126" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
     </row>
     <row r="127">
@@ -1695,7 +1692,7 @@
         <v>72</v>
       </c>
       <c r="B127" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128">
@@ -1703,7 +1700,7 @@
         <v>72</v>
       </c>
       <c r="B128" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
     </row>
     <row r="129">
@@ -1727,7 +1724,7 @@
         <v>72</v>
       </c>
       <c r="B131" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="132">
@@ -1735,7 +1732,7 @@
         <v>72</v>
       </c>
       <c r="B132" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
     </row>
     <row r="133">
@@ -1743,7 +1740,7 @@
         <v>72</v>
       </c>
       <c r="B133" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
     </row>
     <row r="134">
@@ -1751,7 +1748,7 @@
         <v>72</v>
       </c>
       <c r="B134" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="135">
@@ -1759,7 +1756,7 @@
         <v>72</v>
       </c>
       <c r="B135" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="136">
@@ -1767,7 +1764,7 @@
         <v>72</v>
       </c>
       <c r="B136" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="137">
@@ -1775,7 +1772,7 @@
         <v>72</v>
       </c>
       <c r="B137" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
     </row>
     <row r="138">
@@ -1783,7 +1780,7 @@
         <v>72</v>
       </c>
       <c r="B138" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
     </row>
     <row r="139">
@@ -1791,7 +1788,7 @@
         <v>72</v>
       </c>
       <c r="B139" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="140">
@@ -1799,7 +1796,7 @@
         <v>72</v>
       </c>
       <c r="B140" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="141">
@@ -1807,7 +1804,7 @@
         <v>72</v>
       </c>
       <c r="B141" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="142">
@@ -1815,7 +1812,7 @@
         <v>72</v>
       </c>
       <c r="B142" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="143">
@@ -1823,7 +1820,7 @@
         <v>72</v>
       </c>
       <c r="B143" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
     </row>
     <row r="144">
@@ -1831,7 +1828,7 @@
         <v>72</v>
       </c>
       <c r="B144" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
     </row>
     <row r="145">
@@ -1839,7 +1836,7 @@
         <v>72</v>
       </c>
       <c r="B145" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="146">
@@ -1847,7 +1844,7 @@
         <v>72</v>
       </c>
       <c r="B146" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
     </row>
     <row r="147">
@@ -1855,7 +1852,7 @@
         <v>72</v>
       </c>
       <c r="B147" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
     </row>
     <row r="148">
@@ -1863,7 +1860,7 @@
         <v>72</v>
       </c>
       <c r="B148" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="149">
@@ -1871,7 +1868,7 @@
         <v>72</v>
       </c>
       <c r="B149" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="150">
@@ -1879,7 +1876,7 @@
         <v>72</v>
       </c>
       <c r="B150" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="151">
@@ -1887,7 +1884,7 @@
         <v>72</v>
       </c>
       <c r="B151" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
     </row>
     <row r="152">
@@ -1895,7 +1892,7 @@
         <v>72</v>
       </c>
       <c r="B152" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
     </row>
     <row r="153">
@@ -1919,7 +1916,7 @@
         <v>72</v>
       </c>
       <c r="B155" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
     </row>
     <row r="156">
@@ -1927,7 +1924,7 @@
         <v>72</v>
       </c>
       <c r="B156" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
     </row>
     <row r="157">
@@ -1935,7 +1932,7 @@
         <v>72</v>
       </c>
       <c r="B157" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
     </row>
     <row r="158">
@@ -1943,7 +1940,7 @@
         <v>72</v>
       </c>
       <c r="B158" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="159">
@@ -1951,7 +1948,7 @@
         <v>72</v>
       </c>
       <c r="B159" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="160">
@@ -1959,7 +1956,7 @@
         <v>72</v>
       </c>
       <c r="B160" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
     </row>
     <row r="161">
@@ -1967,7 +1964,7 @@
         <v>72</v>
       </c>
       <c r="B161" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
     </row>
     <row r="162">
@@ -1975,7 +1972,7 @@
         <v>72</v>
       </c>
       <c r="B162" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="163">
@@ -1983,7 +1980,7 @@
         <v>72</v>
       </c>
       <c r="B163" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="164">
@@ -1991,7 +1988,7 @@
         <v>72</v>
       </c>
       <c r="B164" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="165">
@@ -1999,7 +1996,7 @@
         <v>72</v>
       </c>
       <c r="B165" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
     </row>
     <row r="166">
@@ -2007,7 +2004,7 @@
         <v>72</v>
       </c>
       <c r="B166" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
     </row>
     <row r="167">
@@ -2015,7 +2012,7 @@
         <v>72</v>
       </c>
       <c r="B167" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="168">
@@ -2023,7 +2020,7 @@
         <v>72</v>
       </c>
       <c r="B168" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
     </row>
     <row r="169">
@@ -2031,7 +2028,7 @@
         <v>72</v>
       </c>
       <c r="B169" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
     </row>
     <row r="170">
@@ -2039,7 +2036,7 @@
         <v>72</v>
       </c>
       <c r="B170" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="171">
@@ -2047,7 +2044,7 @@
         <v>72</v>
       </c>
       <c r="B171" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
     </row>
     <row r="172">
@@ -2063,7 +2060,7 @@
         <v>72</v>
       </c>
       <c r="B173" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
     </row>
     <row r="174">
@@ -2071,7 +2068,7 @@
         <v>72</v>
       </c>
       <c r="B174" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="175">
@@ -2079,7 +2076,7 @@
         <v>72</v>
       </c>
       <c r="B175" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="176">
@@ -2087,7 +2084,7 @@
         <v>72</v>
       </c>
       <c r="B176" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
     </row>
     <row r="177">
@@ -2095,7 +2092,7 @@
         <v>72</v>
       </c>
       <c r="B177" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
     </row>
     <row r="178">
@@ -2103,7 +2100,7 @@
         <v>72</v>
       </c>
       <c r="B178" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="179">
@@ -2111,7 +2108,7 @@
         <v>72</v>
       </c>
       <c r="B179" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="180">
@@ -2119,7 +2116,7 @@
         <v>72</v>
       </c>
       <c r="B180" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="181">
@@ -2127,7 +2124,7 @@
         <v>72</v>
       </c>
       <c r="B181" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="182">
@@ -2135,7 +2132,7 @@
         <v>72</v>
       </c>
       <c r="B182" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
     </row>
     <row r="183">
@@ -2143,7 +2140,7 @@
         <v>72</v>
       </c>
       <c r="B183" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="184">
@@ -2151,28 +2148,28 @@
         <v>72</v>
       </c>
       <c r="B184" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="B185" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="s">
+        <v>93</v>
+      </c>
+      <c r="B186" t="s">
         <v>94</v>
-      </c>
-      <c r="B186" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B187" t="s">
         <v>95</v>
@@ -2180,287 +2177,287 @@
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B188" t="s">
-        <v>96</v>
+        <v>4</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B189" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B190" t="s">
-        <v>97</v>
+        <v>5</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B191" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B192" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B193" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B194" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B195" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B196" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B197" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B198" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B199" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B200" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B201" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B202" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B203" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B204" t="s">
-        <v>18</v>
+        <v>99</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B205" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B206" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B207" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B208" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B209" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B210" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B211" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B212" t="s">
-        <v>101</v>
+        <v>24</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B213" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B214" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B215" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B216" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B217" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B218" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B219" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B220" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B221" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B222" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B223" t="s">
         <v>85</v>
@@ -2468,673 +2465,665 @@
     </row>
     <row r="224">
       <c r="A224" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B224" t="s">
-        <v>86</v>
+        <v>38</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B225" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B226" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B227" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B228" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B229" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B230" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B231" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B232" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B233" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B234" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B235" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B236" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B237" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B238" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B239" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B240" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B241" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B242" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B243" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B244" t="s">
-        <v>104</v>
+        <v>52</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B245" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B246" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B247" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B248" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B249" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B250" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B251" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B252" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B253" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="s">
+        <v>105</v>
+      </c>
+      <c r="B254" t="s">
         <v>106</v>
-      </c>
-      <c r="B254" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B255" t="s">
-        <v>107</v>
+        <v>5</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B256" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B257" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B258" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B259" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B260" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B261" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B262" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B263" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B264" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B265" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B266" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B267" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B268" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B269" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B270" t="s">
-        <v>18</v>
+        <v>99</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B271" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B272" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B273" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B274" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B275" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B276" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B277" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B278" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B279" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B280" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B281" t="s">
-        <v>110</v>
+        <v>36</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B282" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B283" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B284" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B285" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B286" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B287" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B288" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B289" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B290" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B291" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B292" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B293" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B294" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B295" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B296" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B297" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B298" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B299" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B300" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B301" t="s">
-        <v>104</v>
+        <v>52</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B302" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B303" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B304" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B305" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B306" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="307">
-      <c r="A307" t="s">
-        <v>106</v>
-      </c>
-      <c r="B307" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
now ingesting csv instead of json
</commit_message>
<xml_diff>
--- a/data/01 application country names per year.xlsx
+++ b/data/01 application country names per year.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>project_year</t>
   </si>
@@ -300,9 +300,6 @@
   </si>
   <si>
     <t>Armenia</t>
-  </si>
-  <si>
-    <t>Bahrain</t>
   </si>
   <si>
     <t>Benin</t>
@@ -2188,7 +2185,7 @@
         <v>93</v>
       </c>
       <c r="B189" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
     </row>
     <row r="190">
@@ -2196,7 +2193,7 @@
         <v>93</v>
       </c>
       <c r="B190" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
     </row>
     <row r="191">
@@ -2204,7 +2201,7 @@
         <v>93</v>
       </c>
       <c r="B191" t="s">
-        <v>97</v>
+        <v>9</v>
       </c>
     </row>
     <row r="192">
@@ -2212,7 +2209,7 @@
         <v>93</v>
       </c>
       <c r="B192" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="193">
@@ -2220,7 +2217,7 @@
         <v>93</v>
       </c>
       <c r="B193" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="194">
@@ -2228,7 +2225,7 @@
         <v>93</v>
       </c>
       <c r="B194" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="195">
@@ -2236,7 +2233,7 @@
         <v>93</v>
       </c>
       <c r="B195" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196">
@@ -2244,7 +2241,7 @@
         <v>93</v>
       </c>
       <c r="B196" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="197">
@@ -2252,7 +2249,7 @@
         <v>93</v>
       </c>
       <c r="B197" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
     </row>
     <row r="198">
@@ -2260,7 +2257,7 @@
         <v>93</v>
       </c>
       <c r="B198" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="199">
@@ -2268,7 +2265,7 @@
         <v>93</v>
       </c>
       <c r="B199" t="s">
-        <v>77</v>
+        <v>16</v>
       </c>
     </row>
     <row r="200">
@@ -2276,7 +2273,7 @@
         <v>93</v>
       </c>
       <c r="B200" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="201">
@@ -2284,7 +2281,7 @@
         <v>93</v>
       </c>
       <c r="B201" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
     </row>
     <row r="202">
@@ -2292,7 +2289,7 @@
         <v>93</v>
       </c>
       <c r="B202" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
     </row>
     <row r="203">
@@ -2300,7 +2297,7 @@
         <v>93</v>
       </c>
       <c r="B203" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
     </row>
     <row r="204">
@@ -2308,7 +2305,7 @@
         <v>93</v>
       </c>
       <c r="B204" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
     </row>
     <row r="205">
@@ -2316,7 +2313,7 @@
         <v>93</v>
       </c>
       <c r="B205" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="206">
@@ -2324,7 +2321,7 @@
         <v>93</v>
       </c>
       <c r="B206" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
     </row>
     <row r="207">
@@ -2332,7 +2329,7 @@
         <v>93</v>
       </c>
       <c r="B207" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="208">
@@ -2340,7 +2337,7 @@
         <v>93</v>
       </c>
       <c r="B208" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="209">
@@ -2348,7 +2345,7 @@
         <v>93</v>
       </c>
       <c r="B209" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
     </row>
     <row r="210">
@@ -2356,7 +2353,7 @@
         <v>93</v>
       </c>
       <c r="B210" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
     </row>
     <row r="211">
@@ -2364,7 +2361,7 @@
         <v>93</v>
       </c>
       <c r="B211" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
     </row>
     <row r="212">
@@ -2372,7 +2369,7 @@
         <v>93</v>
       </c>
       <c r="B212" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="213">
@@ -2380,7 +2377,7 @@
         <v>93</v>
       </c>
       <c r="B213" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="214">
@@ -2388,7 +2385,7 @@
         <v>93</v>
       </c>
       <c r="B214" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="215">
@@ -2396,7 +2393,7 @@
         <v>93</v>
       </c>
       <c r="B215" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="216">
@@ -2404,7 +2401,7 @@
         <v>93</v>
       </c>
       <c r="B216" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
     </row>
     <row r="217">
@@ -2412,7 +2409,7 @@
         <v>93</v>
       </c>
       <c r="B217" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
     </row>
     <row r="218">
@@ -2420,7 +2417,7 @@
         <v>93</v>
       </c>
       <c r="B218" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="219">
@@ -2428,7 +2425,7 @@
         <v>93</v>
       </c>
       <c r="B219" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="220">
@@ -2436,7 +2433,7 @@
         <v>93</v>
       </c>
       <c r="B220" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="221">
@@ -2444,7 +2441,7 @@
         <v>93</v>
       </c>
       <c r="B221" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
     </row>
     <row r="222">
@@ -2452,7 +2449,7 @@
         <v>93</v>
       </c>
       <c r="B222" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="223">
@@ -2460,7 +2457,7 @@
         <v>93</v>
       </c>
       <c r="B223" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
     </row>
     <row r="224">
@@ -2468,7 +2465,7 @@
         <v>93</v>
       </c>
       <c r="B224" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="225">
@@ -2476,7 +2473,7 @@
         <v>93</v>
       </c>
       <c r="B225" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="226">
@@ -2484,7 +2481,7 @@
         <v>93</v>
       </c>
       <c r="B226" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
     </row>
     <row r="227">
@@ -2492,7 +2489,7 @@
         <v>93</v>
       </c>
       <c r="B227" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="228">
@@ -2500,7 +2497,7 @@
         <v>93</v>
       </c>
       <c r="B228" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
     </row>
     <row r="229">
@@ -2508,7 +2505,7 @@
         <v>93</v>
       </c>
       <c r="B229" t="s">
-        <v>101</v>
+        <v>42</v>
       </c>
     </row>
     <row r="230">
@@ -2516,7 +2513,7 @@
         <v>93</v>
       </c>
       <c r="B230" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="231">
@@ -2524,7 +2521,7 @@
         <v>93</v>
       </c>
       <c r="B231" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="232">
@@ -2532,7 +2529,7 @@
         <v>93</v>
       </c>
       <c r="B232" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="233">
@@ -2540,7 +2537,7 @@
         <v>93</v>
       </c>
       <c r="B233" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="234">
@@ -2548,7 +2545,7 @@
         <v>93</v>
       </c>
       <c r="B234" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="235">
@@ -2556,7 +2553,7 @@
         <v>93</v>
       </c>
       <c r="B235" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="236">
@@ -2564,7 +2561,7 @@
         <v>93</v>
       </c>
       <c r="B236" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
     </row>
     <row r="237">
@@ -2572,7 +2569,7 @@
         <v>93</v>
       </c>
       <c r="B237" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
     </row>
     <row r="238">
@@ -2580,7 +2577,7 @@
         <v>93</v>
       </c>
       <c r="B238" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="239">
@@ -2588,7 +2585,7 @@
         <v>93</v>
       </c>
       <c r="B239" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
     </row>
     <row r="240">
@@ -2596,7 +2593,7 @@
         <v>93</v>
       </c>
       <c r="B240" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="241">
@@ -2604,7 +2601,7 @@
         <v>93</v>
       </c>
       <c r="B241" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
     </row>
     <row r="242">
@@ -2612,7 +2609,7 @@
         <v>93</v>
       </c>
       <c r="B242" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
     </row>
     <row r="243">
@@ -2620,7 +2617,7 @@
         <v>93</v>
       </c>
       <c r="B243" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
     </row>
     <row r="244">
@@ -2628,7 +2625,7 @@
         <v>93</v>
       </c>
       <c r="B244" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
     </row>
     <row r="245">
@@ -2636,7 +2633,7 @@
         <v>93</v>
       </c>
       <c r="B245" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
     </row>
     <row r="246">
@@ -2644,7 +2641,7 @@
         <v>93</v>
       </c>
       <c r="B246" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="247">
@@ -2652,7 +2649,7 @@
         <v>93</v>
       </c>
       <c r="B247" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="248">
@@ -2660,7 +2657,7 @@
         <v>93</v>
       </c>
       <c r="B248" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
     </row>
     <row r="249">
@@ -2668,7 +2665,7 @@
         <v>93</v>
       </c>
       <c r="B249" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="250">
@@ -2676,454 +2673,446 @@
         <v>93</v>
       </c>
       <c r="B250" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B251" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B252" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="s">
+        <v>104</v>
+      </c>
+      <c r="B253" t="s">
         <v>105</v>
-      </c>
-      <c r="B253" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B254" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B255" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B256" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B257" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B258" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B259" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B260" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B261" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B262" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B263" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B264" t="s">
-        <v>108</v>
+        <v>15</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B265" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B266" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B267" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B268" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B269" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B270" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B271" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B272" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B273" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B274" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B275" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B276" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B277" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B278" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B279" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B280" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B281" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B282" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B283" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B284" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B285" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B286" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B287" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B288" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B289" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B290" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B291" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B292" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B293" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B294" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B295" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B296" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B297" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B298" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B299" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B300" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B301" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B302" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B303" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B304" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B305" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="306">
-      <c r="A306" t="s">
-        <v>105</v>
-      </c>
-      <c r="B306" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>